<commit_message>
shortlisted data fetchingin excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
     <sheet name="shortlisted" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:T18"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>source</t>
   </si>
@@ -173,45 +173,131 @@
     <t>rahu#l@gmail.com</t>
   </si>
   <si>
-    <t>ddfd</t>
-  </si>
-  <si>
-    <t>effdshgjs@wdgwj.ksdh</t>
-  </si>
-  <si>
-    <t>47836836</t>
-  </si>
-  <si>
     <t>candidateEmail</t>
   </si>
   <si>
     <t>contactNumber</t>
   </si>
   <si>
-    <t>whatsupNumber</t>
-  </si>
-  <si>
-    <t>sourceName</t>
-  </si>
-  <si>
-    <t>callingRemark</t>
-  </si>
-  <si>
-    <t>9176576576</t>
+    <t>whatappNumber</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>callingFeedback</t>
+  </si>
+  <si>
+    <t>D.O.B</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>callSummary</t>
+  </si>
+  <si>
+    <t>passout</t>
+  </si>
+  <si>
+    <t>certification</t>
+  </si>
+  <si>
+    <t>CurrentCompany</t>
+  </si>
+  <si>
+    <t>TotalExp</t>
+  </si>
+  <si>
+    <t>communication Rating</t>
+  </si>
+  <si>
+    <t>current CTC</t>
+  </si>
+  <si>
+    <t>expected CTC</t>
+  </si>
+  <si>
+    <t>offer Letter</t>
+  </si>
+  <si>
+    <t>offer letter message</t>
+  </si>
+  <si>
+    <t>message for TL</t>
+  </si>
+  <si>
+    <t>status Type</t>
+  </si>
+  <si>
+    <t>final status</t>
+  </si>
+  <si>
+    <t>interview Date</t>
+  </si>
+  <si>
+    <t>interview Time</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>26</t>
+    <t>rani@yahoo.com</t>
+  </si>
+  <si>
+    <t>JAVA,SQL</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>GOOD</t>
+  </si>
+  <si>
+    <t>32 - Data Analyst</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Rani@gmail.com</t>
+  </si>
+  <si>
+    <t>918080888889</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>suma</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Interview Schedule</t>
+  </si>
+  <si>
+    <t>2 year,2 month</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> year, month</t>
+  </si>
+  <si>
+    <t>BCA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,13 +335,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -286,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -295,6 +395,8 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,29 +685,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N3" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="14.42578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="5" max="5" customWidth="true" width="12.42578125"/>
-    <col min="6" max="6" customWidth="true" width="11.7109375"/>
-    <col min="7" max="7" customWidth="true" width="20.140625"/>
-    <col min="10" max="10" customWidth="true" width="9.85546875"/>
-    <col min="11" max="11" customWidth="true" width="14.140625"/>
-    <col min="12" max="12" customWidth="true" width="12.28515625"/>
-    <col min="13" max="13" customWidth="true" width="13.5703125"/>
-    <col min="14" max="14" customWidth="true" width="11.85546875"/>
-    <col min="15" max="15" customWidth="true" width="12.0"/>
-    <col min="16" max="16" customWidth="true" width="14.42578125"/>
-    <col min="17" max="17" customWidth="true" width="10.85546875"/>
-    <col min="18" max="18" customWidth="true" width="11.85546875"/>
-    <col min="19" max="19" customWidth="true" width="10.42578125"/>
-    <col min="20" max="20" customWidth="true" width="23.0"/>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -861,115 +963,328 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.28515625"/>
-    <col min="2" max="2" customWidth="true" width="21.0"/>
-    <col min="3" max="3" customWidth="true" width="14.140625"/>
-    <col min="4" max="4" customWidth="true" width="15.140625"/>
-    <col min="5" max="5" customWidth="true" width="11.42578125"/>
-    <col min="7" max="7" customWidth="true" width="12.7109375"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="25" max="25" width="26.7109375" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="L1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" t="s">
+        <v>88</v>
+      </c>
+      <c r="U2" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="R3" s="1">
+        <v>15</v>
+      </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the recruiter script
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
     <sheet name="shortlisted" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="P1:Y18"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
   <si>
     <t>source</t>
   </si>
@@ -164,9 +164,6 @@
     <t>23 - HR Recruiter</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>MCA</t>
   </si>
   <si>
@@ -242,15 +239,9 @@
     <t/>
   </si>
   <si>
-    <t>rani@yahoo.com</t>
-  </si>
-  <si>
     <t>JAVA,SQL</t>
   </si>
   <si>
-    <t>3,4</t>
-  </si>
-  <si>
     <t>GOOD</t>
   </si>
   <si>
@@ -260,43 +251,94 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Rani@gmail.com</t>
-  </si>
-  <si>
-    <t>918080888889</t>
-  </si>
-  <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>suma</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Interview Schedule</t>
   </si>
   <si>
-    <t>2 year,2 month</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> year, month</t>
-  </si>
-  <si>
     <t>BCA</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>interviewDate</t>
+  </si>
+  <si>
+    <t>interviewTime</t>
+  </si>
+  <si>
+    <t>2:20</t>
+  </si>
+  <si>
+    <t>EXCELLENT</t>
+  </si>
+  <si>
+    <t>3 year,5 month</t>
+  </si>
+  <si>
+    <t>wipro</t>
+  </si>
+  <si>
+    <t>rahu</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2 year,6 month</t>
+  </si>
+  <si>
+    <t>4 year,5 month</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Msys Technologies</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>2 Lakh,6 Thousand</t>
+  </si>
+  <si>
+    <t>4 Lakh,5 Thousand</t>
+  </si>
+  <si>
+    <t>1233211238</t>
+  </si>
+  <si>
+    <t>0010-02-26</t>
+  </si>
+  <si>
+    <t>rani123@yahoo.com</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>JAVA,SQL,manual</t>
+  </si>
+  <si>
+    <t>excellent</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>take it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -397,6 +439,10 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -683,34 +729,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView topLeftCell="N3" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125"/>
+    <col min="6" max="6" customWidth="true" width="11.7109375"/>
+    <col min="7" max="7" customWidth="true" width="20.140625"/>
+    <col min="10" max="10" customWidth="true" width="9.85546875"/>
+    <col min="11" max="11" customWidth="true" width="14.140625"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625"/>
+    <col min="13" max="13" customWidth="true" width="13.5703125"/>
+    <col min="14" max="14" customWidth="true" width="11.85546875"/>
+    <col min="15" max="15" customWidth="true" width="12.0"/>
+    <col min="16" max="16" customWidth="true" width="14.42578125"/>
+    <col min="17" max="17" customWidth="true" width="10.85546875"/>
+    <col min="18" max="18" customWidth="true" width="11.85546875"/>
+    <col min="19" max="19" customWidth="true" width="10.42578125"/>
+    <col min="20" max="20" customWidth="true" width="23.0"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -771,8 +818,17 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -831,8 +887,11 @@
       <c r="T2" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -867,13 +926,16 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>38</v>
@@ -897,9 +959,7 @@
       <c r="J4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>48</v>
-      </c>
+      <c r="K4" s="6"/>
       <c r="L4" s="6">
         <v>1</v>
       </c>
@@ -927,8 +987,15 @@
       <c r="T4" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="U4" s="11">
+        <v>37644</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="12" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
@@ -949,6 +1016,9 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -965,37 +1035,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" customWidth="1"/>
-    <col min="25" max="25" width="26.7109375" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="28" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875"/>
+    <col min="7" max="7" customWidth="true" width="11.85546875"/>
+    <col min="8" max="8" customWidth="true" width="16.140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="11" max="11" customWidth="true" width="13.7109375"/>
+    <col min="12" max="12" customWidth="true" width="12.5703125"/>
+    <col min="14" max="14" customWidth="true" width="14.5703125"/>
+    <col min="15" max="15" customWidth="true" width="18.28515625"/>
+    <col min="16" max="16" customWidth="true" width="13.140625"/>
+    <col min="17" max="17" customWidth="true" width="11.7109375"/>
+    <col min="18" max="18" customWidth="true" width="12.140625"/>
+    <col min="19" max="19" customWidth="true" width="20.7109375"/>
+    <col min="20" max="20" customWidth="true" width="11.0"/>
+    <col min="21" max="21" customWidth="true" width="13.0"/>
+    <col min="22" max="22" customWidth="true" width="11.42578125"/>
+    <col min="23" max="23" customWidth="true" width="19.140625"/>
+    <col min="24" max="24" customWidth="true" width="15.5703125"/>
+    <col min="25" max="25" customWidth="true" width="26.7109375"/>
+    <col min="26" max="26" customWidth="true" width="19.42578125"/>
+    <col min="27" max="27" customWidth="true" width="14.85546875"/>
+    <col min="28" max="28" customWidth="true" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1003,13 +1074,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>0</v>
@@ -1018,34 +1089,34 @@
         <v>6</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>19</v>
@@ -1054,168 +1125,186 @@
         <v>13</v>
       </c>
       <c r="S1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="Q2" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="S2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="O2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="U2" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="W2" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="R2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" t="s">
-        <v>88</v>
-      </c>
-      <c r="U2" t="s">
-        <v>88</v>
-      </c>
-      <c r="V2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>72</v>
-      </c>
+      <c r="X2" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="Z2" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="AA2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="0"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123321123</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="13">
+        <v>36809</v>
+      </c>
       <c r="J3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2024</v>
+      </c>
       <c r="N3" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q3" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>3</v>
+      </c>
       <c r="R3" s="1">
         <v>15</v>
       </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="X3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y3" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>

</xml_diff>

<commit_message>
updated as sir needed the new data to be calculated
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="8370" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="lineUpTracker" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P18"/>
+  <oleSize ref="Q1:Z18"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="115">
   <si>
     <t>source</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>0022-09-19</t>
+  </si>
+  <si>
+    <t>rani123#@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -480,6 +482,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -768,30 +771,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="14.42578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="5" max="5" customWidth="true" width="12.42578125"/>
-    <col min="6" max="6" customWidth="true" width="11.7109375"/>
-    <col min="7" max="7" customWidth="true" width="20.140625"/>
-    <col min="10" max="10" customWidth="true" width="9.85546875"/>
-    <col min="11" max="11" customWidth="true" width="14.140625"/>
-    <col min="12" max="12" customWidth="true" width="12.28515625"/>
-    <col min="13" max="13" customWidth="true" width="13.5703125"/>
-    <col min="14" max="14" customWidth="true" width="11.85546875"/>
-    <col min="15" max="15" customWidth="true" width="12.0"/>
-    <col min="16" max="16" customWidth="true" width="14.42578125"/>
-    <col min="17" max="17" customWidth="true" width="10.85546875"/>
-    <col min="18" max="18" customWidth="true" width="11.85546875"/>
-    <col min="19" max="19" customWidth="true" width="10.42578125"/>
-    <col min="20" max="20" customWidth="true" width="23.0"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -855,13 +858,13 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="9" t="s">
         <v>77</v>
       </c>
     </row>
@@ -869,7 +872,7 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -932,7 +935,7 @@
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -968,67 +971,67 @@
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>3232132321</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5">
         <v>1</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>2</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>1</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="6">
         <v>240000</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>300000</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="S4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="11">
+      <c r="U4" s="10">
         <v>37644</v>
       </c>
       <c r="V4" s="1"/>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="11" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1073,211 +1076,211 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection sqref="A1:AB5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.7109375"/>
-    <col min="2" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="12.7109375"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375"/>
-    <col min="5" max="5" customWidth="true" width="13.42578125"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875"/>
-    <col min="7" max="7" customWidth="true" width="11.85546875"/>
-    <col min="8" max="8" customWidth="true" width="16.140625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
-    <col min="11" max="11" customWidth="true" width="13.7109375"/>
-    <col min="12" max="12" customWidth="true" width="12.5703125"/>
-    <col min="14" max="14" customWidth="true" width="14.5703125"/>
-    <col min="15" max="15" customWidth="true" width="18.28515625"/>
-    <col min="16" max="16" customWidth="true" width="13.140625"/>
-    <col min="17" max="17" customWidth="true" width="11.7109375"/>
-    <col min="18" max="18" customWidth="true" width="12.140625"/>
-    <col min="19" max="19" customWidth="true" width="20.7109375"/>
-    <col min="20" max="20" customWidth="true" width="11.0"/>
-    <col min="21" max="21" customWidth="true" width="13.0"/>
-    <col min="22" max="22" customWidth="true" width="11.42578125"/>
-    <col min="23" max="23" customWidth="true" width="19.140625"/>
-    <col min="24" max="24" customWidth="true" width="15.5703125"/>
-    <col min="25" max="25" customWidth="true" width="26.7109375"/>
-    <col min="26" max="26" customWidth="true" width="19.42578125"/>
-    <col min="27" max="27" customWidth="true" width="14.85546875"/>
-    <col min="28" max="28" customWidth="true" width="14.0"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="25" max="25" width="26.7109375" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>92</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
         <v>94</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>97</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>95</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" t="s" s="0">
+      <c r="Q2" t="s">
         <v>87</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="R2" t="s">
         <v>88</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>79</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>89</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>90</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>29</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>81</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" t="s" s="0">
+      <c r="Z2" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" t="s" s="0">
+      <c r="AA2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="1">
@@ -1294,7 +1297,7 @@
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>36809</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1408,9 +1411,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1424,176 +1428,176 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>107</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s" s="0">
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
         <v>110</v>
       </c>
-      <c r="I2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="M2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="N2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
         <v>99</v>
       </c>
-      <c r="Q2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="R2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="T2" t="s" s="0">
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
         <v>100</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>100</v>
       </c>
-      <c r="V2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="W2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="X2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="Y2" t="s" s="0">
+      <c r="V2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="AA2" t="s" s="0">
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1601,22 +1605,22 @@
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C3" s="1">
         <v>2312312311</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1640,7 +1644,7 @@
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" t="s" s="0">
+      <c r="Y3" t="s">
         <v>38</v>
       </c>
       <c r="Z3" s="1" t="s">
@@ -1692,190 +1696,189 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>112</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>105</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>113</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
         <v>94</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>97</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>95</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" t="s" s="0">
+      <c r="Q2" t="s">
         <v>87</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="R2" t="s">
         <v>88</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>79</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>89</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>90</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>29</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>111</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>96</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" t="s" s="0">
+      <c r="Z2" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="AB2" s="0"/>
+      <c r="AA2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>112</v>
       </c>
       <c r="C3" s="1"/>
@@ -1890,7 +1893,7 @@
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>

</xml_diff>

<commit_message>
class added to check the status of hold candidate
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="6180" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
     <sheet name="shortlisted" sheetId="3" r:id="rId2"/>
     <sheet name="callingTracker" sheetId="4" r:id="rId3"/>
     <sheet name="lineUpTracker" sheetId="5" r:id="rId4"/>
+    <sheet name="Hold Candidate" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="Q1:Z18"/>
+  <oleSize ref="A1:L18"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4590" uniqueCount="158">
   <si>
     <t>source</t>
   </si>
@@ -368,6 +369,135 @@
   </si>
   <si>
     <t>rani123#@yahoo.com</t>
+  </si>
+  <si>
+    <t>Candidate Name</t>
+  </si>
+  <si>
+    <t>Candidate Email</t>
+  </si>
+  <si>
+    <t>contact Number</t>
+  </si>
+  <si>
+    <t>alternate Number</t>
+  </si>
+  <si>
+    <t>source Name</t>
+  </si>
+  <si>
+    <t>job Id</t>
+  </si>
+  <si>
+    <t>job Designation</t>
+  </si>
+  <si>
+    <t>requirement Company</t>
+  </si>
+  <si>
+    <t>current Location</t>
+  </si>
+  <si>
+    <t>full Address</t>
+  </si>
+  <si>
+    <t>calling Feedback</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>Saddam Kazi</t>
+  </si>
+  <si>
+    <t>91123456789</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>157 industries</t>
+  </si>
+  <si>
+    <t>Yeshawant Nagar Malkapur</t>
+  </si>
+  <si>
+    <t>2000-10-10</t>
+  </si>
+  <si>
+    <t>feedBack</t>
+  </si>
+  <si>
+    <t>Current Company</t>
+  </si>
+  <si>
+    <t>Total Experience</t>
+  </si>
+  <si>
+    <t>Relevent Experience</t>
+  </si>
+  <si>
+    <t>Notice Period</t>
+  </si>
+  <si>
+    <t>Communication Rating</t>
+  </si>
+  <si>
+    <t>Current CTC</t>
+  </si>
+  <si>
+    <t>Expected CTC</t>
+  </si>
+  <si>
+    <t>OfferLetter Msg</t>
+  </si>
+  <si>
+    <t>messageFor TL</t>
+  </si>
+  <si>
+    <t>finalStatus</t>
+  </si>
+  <si>
+    <t>Interviewdate</t>
+  </si>
+  <si>
+    <t>InterviewTime</t>
+  </si>
+  <si>
+    <t>Associate of Science (AS)</t>
+  </si>
+  <si>
+    <t>Full Stack Certificate</t>
+  </si>
+  <si>
+    <t>Telious Technologies Pvt Ltd Kochi, Kerala</t>
+  </si>
+  <si>
+    <t>10 year,1 month</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>30 Days</t>
+  </si>
+  <si>
+    <t>8 good</t>
+  </si>
+  <si>
+    <t>11 Lakh,11 Thousand</t>
+  </si>
+  <si>
+    <t>34 Lakh,34 Thousand</t>
+  </si>
+  <si>
+    <t>hee is holding wipro letter</t>
+  </si>
+  <si>
+    <t>Good Candidate</t>
+  </si>
+  <si>
+    <t>2024-10-21</t>
   </si>
 </sst>
 </file>
@@ -771,30 +901,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125"/>
+    <col min="6" max="6" customWidth="true" width="11.7109375"/>
+    <col min="7" max="7" customWidth="true" width="20.140625"/>
+    <col min="10" max="10" customWidth="true" width="9.85546875"/>
+    <col min="11" max="11" customWidth="true" width="14.140625"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625"/>
+    <col min="13" max="13" customWidth="true" width="13.5703125"/>
+    <col min="14" max="14" customWidth="true" width="11.85546875"/>
+    <col min="15" max="15" customWidth="true" width="12.0"/>
+    <col min="16" max="16" customWidth="true" width="14.42578125"/>
+    <col min="17" max="17" customWidth="true" width="10.85546875"/>
+    <col min="18" max="18" customWidth="true" width="11.85546875"/>
+    <col min="19" max="19" customWidth="true" width="10.42578125"/>
+    <col min="20" max="20" customWidth="true" width="23.0"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -1081,32 +1211,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" customWidth="1"/>
-    <col min="25" max="25" width="26.7109375" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="28" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875"/>
+    <col min="7" max="7" customWidth="true" width="11.85546875"/>
+    <col min="8" max="8" customWidth="true" width="16.140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="11" max="11" customWidth="true" width="13.7109375"/>
+    <col min="12" max="12" customWidth="true" width="12.5703125"/>
+    <col min="14" max="14" customWidth="true" width="14.5703125"/>
+    <col min="15" max="15" customWidth="true" width="18.28515625"/>
+    <col min="16" max="16" customWidth="true" width="13.140625"/>
+    <col min="17" max="17" customWidth="true" width="11.7109375"/>
+    <col min="18" max="18" customWidth="true" width="12.140625"/>
+    <col min="19" max="19" customWidth="true" width="20.7109375"/>
+    <col min="20" max="20" customWidth="true" width="11.0"/>
+    <col min="21" max="21" customWidth="true" width="13.0"/>
+    <col min="22" max="22" customWidth="true" width="11.42578125"/>
+    <col min="23" max="23" customWidth="true" width="19.140625"/>
+    <col min="24" max="24" customWidth="true" width="15.5703125"/>
+    <col min="25" max="25" customWidth="true" width="26.7109375"/>
+    <col min="26" max="26" customWidth="true" width="19.42578125"/>
+    <col min="27" max="27" customWidth="true" width="14.85546875"/>
+    <col min="28" max="28" customWidth="true" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1196,85 +1326,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>82</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -1428,8 +1558,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1519,85 +1649,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="I2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="Q2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="Q2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="V2" t="s">
-        <v>71</v>
-      </c>
-      <c r="W2" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="V2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="Z2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="Z2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AA2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -1612,12 +1742,12 @@
         <v>2312312311</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>22</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>23</v>
       </c>
       <c r="I3" s="13"/>
@@ -1644,7 +1774,7 @@
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" t="s">
+      <c r="Y3" t="s" s="0">
         <v>38</v>
       </c>
       <c r="Z3" s="1" t="s">
@@ -1702,7 +1832,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1792,85 +1922,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -2007,4 +2137,207 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AE3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="Q2" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="T2" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="U2" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="W2" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="X2" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="Z2" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="AA2" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="AB2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="AC2" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="AD2" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="AE2" t="s" s="0">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="Q3" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="R3" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="S3" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="T3" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="U3" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="V3" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="W3" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="X3" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="Y3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Z3" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="AA3" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="AB3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="AC3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AD3" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="AE3" s="0"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
database added to applicant
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -17,7 +17,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1:L18"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="196">
   <si>
     <t>source</t>
   </si>
@@ -583,6 +583,36 @@
   </si>
   <si>
     <t>BASED ON THE IMPORTANCE</t>
+  </si>
+  <si>
+    <t>a1@gmail.com</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>2005-06-08</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>sql,plsql</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1 Lakh,1 Thousand</t>
+  </si>
+  <si>
+    <t>2 Lakh,2 Thousand</t>
+  </si>
+  <si>
+    <t>2024-12-25</t>
+  </si>
+  <si>
+    <t>a1</t>
   </si>
 </sst>
 </file>
@@ -998,24 +1028,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125"/>
+    <col min="6" max="6" customWidth="true" width="11.7109375"/>
+    <col min="7" max="7" customWidth="true" width="20.140625"/>
+    <col min="10" max="10" customWidth="true" width="9.85546875"/>
+    <col min="11" max="11" customWidth="true" width="14.140625"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625"/>
+    <col min="13" max="13" customWidth="true" width="13.5703125"/>
+    <col min="14" max="14" customWidth="true" width="11.85546875"/>
+    <col min="15" max="15" customWidth="true" width="12.0"/>
+    <col min="16" max="16" customWidth="true" width="14.42578125"/>
+    <col min="17" max="17" customWidth="true" width="10.85546875"/>
+    <col min="18" max="18" customWidth="true" width="11.85546875"/>
+    <col min="19" max="19" customWidth="true" width="10.42578125"/>
+    <col min="20" max="20" customWidth="true" width="23.0"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -1302,32 +1332,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" customWidth="1"/>
-    <col min="25" max="25" width="26.7109375" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="28" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375"/>
+    <col min="2" max="2" customWidth="true" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875"/>
+    <col min="7" max="7" customWidth="true" width="11.85546875"/>
+    <col min="8" max="8" customWidth="true" width="16.140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="11" max="11" customWidth="true" width="13.7109375"/>
+    <col min="12" max="12" customWidth="true" width="12.5703125"/>
+    <col min="14" max="14" customWidth="true" width="14.5703125"/>
+    <col min="15" max="15" customWidth="true" width="18.28515625"/>
+    <col min="16" max="16" customWidth="true" width="13.140625"/>
+    <col min="17" max="17" customWidth="true" width="11.7109375"/>
+    <col min="18" max="18" customWidth="true" width="12.140625"/>
+    <col min="19" max="19" customWidth="true" width="20.7109375"/>
+    <col min="20" max="20" customWidth="true" width="11.0"/>
+    <col min="21" max="21" customWidth="true" width="13.0"/>
+    <col min="22" max="22" customWidth="true" width="11.42578125"/>
+    <col min="23" max="23" customWidth="true" width="19.140625"/>
+    <col min="24" max="24" customWidth="true" width="15.5703125"/>
+    <col min="25" max="25" customWidth="true" width="26.7109375"/>
+    <col min="26" max="26" customWidth="true" width="19.42578125"/>
+    <col min="27" max="27" customWidth="true" width="14.85546875"/>
+    <col min="28" max="28" customWidth="true" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1417,85 +1447,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>82</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -1649,8 +1679,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1740,87 +1770,88 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" t="s">
-        <v>139</v>
-      </c>
-      <c r="N2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="Q2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" t="s">
-        <v>100</v>
-      </c>
-      <c r="U2" t="s">
-        <v>100</v>
-      </c>
-      <c r="V2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>71</v>
-      </c>
+      <c r="Q2" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="U2" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="Z2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AA2" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="AB2" s="0"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1833,12 +1864,12 @@
         <v>2312312311</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>22</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>23</v>
       </c>
       <c r="I3" s="13"/>
@@ -1865,7 +1896,7 @@
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" t="s">
+      <c r="Y3" t="s" s="0">
         <v>137</v>
       </c>
       <c r="Z3" s="1" t="s">
@@ -1923,7 +1954,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2013,85 +2044,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>71</v>
       </c>
     </row>
@@ -2240,222 +2271,222 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.42578125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.42578125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.28515625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="7.28515625"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="23.42578125"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="7.85546875"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="19.28515625"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="38.85546875"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="19.5703125"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="21.42578125"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="19.28515625"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.140625"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="24.85546875"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="15.28515625"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.5703125"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="13.7109375"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>126</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" t="s" s="0">
         <v>134</v>
       </c>
       <c r="AF2" s="15"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="J3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="L3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="O3" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="Q3" t="s">
-        <v>71</v>
-      </c>
-      <c r="R3" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="Q3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="R3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="S3" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="Z3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="Z3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AA3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AB3" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="AC3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD3" t="s">
+      <c r="AC3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="AD3" t="s" s="0">
         <v>71</v>
       </c>
       <c r="AF3" s="1"/>
@@ -2578,152 +2609,152 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.85546875"/>
+    <col min="2" max="2" customWidth="true" width="17.85546875"/>
+    <col min="3" max="3" customWidth="true" width="15.28515625"/>
+    <col min="4" max="4" customWidth="true" width="20.5703125"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375"/>
+    <col min="6" max="6" customWidth="true" width="14.42578125"/>
+    <col min="7" max="7" customWidth="true" width="12.28515625"/>
+    <col min="8" max="8" customWidth="true" width="17.7109375"/>
+    <col min="9" max="9" customWidth="true" width="8.5703125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.7109375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="17.85546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.5703125"/>
+    <col min="15" max="15" customWidth="true" width="8.140625"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.140625"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.140625"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.7109375"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>158</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>162</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>173</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" t="s" s="0">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>8989898989</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>157</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>161</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="0">
         <v>2</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="0">
         <v>3.6</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="s" s="0">
         <v>183</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" t="s" s="0">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel sheet modified as the data got delected
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="8370" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6180" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
     <sheet name="shortlisted" sheetId="3" r:id="rId2"/>
     <sheet name="callingTracker" sheetId="4" r:id="rId3"/>
     <sheet name="lineUpTracker" sheetId="5" r:id="rId4"/>
+    <sheet name="Hold Candidate" sheetId="6" r:id="rId5"/>
+    <sheet name="applicant" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P18"/>
+  <oleSize ref="A1:L18"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="186">
   <si>
     <t>source</t>
   </si>
@@ -343,21 +345,6 @@
     <t>9132321323219</t>
   </si>
   <si>
-    <t>Arshad Attar</t>
-  </si>
-  <si>
-    <t>arshattar36@gmail.com</t>
-  </si>
-  <si>
-    <t>917887755337</t>
-  </si>
-  <si>
-    <t>LinkedIn</t>
-  </si>
-  <si>
-    <t>Call Done</t>
-  </si>
-  <si>
     <t>TCS</t>
   </si>
   <si>
@@ -365,6 +352,237 @@
   </si>
   <si>
     <t>0022-09-19</t>
+  </si>
+  <si>
+    <t>rani123#@yahoo.com</t>
+  </si>
+  <si>
+    <t>Candidate Name</t>
+  </si>
+  <si>
+    <t>Candidate Email</t>
+  </si>
+  <si>
+    <t>contact Number</t>
+  </si>
+  <si>
+    <t>alternate Number</t>
+  </si>
+  <si>
+    <t>source Name</t>
+  </si>
+  <si>
+    <t>job Id</t>
+  </si>
+  <si>
+    <t>job Designation</t>
+  </si>
+  <si>
+    <t>requirement Company</t>
+  </si>
+  <si>
+    <t>current Location</t>
+  </si>
+  <si>
+    <t>full Address</t>
+  </si>
+  <si>
+    <t>calling Feedback</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>feedBack</t>
+  </si>
+  <si>
+    <t>Current Company</t>
+  </si>
+  <si>
+    <t>Total Experience</t>
+  </si>
+  <si>
+    <t>Relevent Experience</t>
+  </si>
+  <si>
+    <t>Notice Period</t>
+  </si>
+  <si>
+    <t>Communication Rating</t>
+  </si>
+  <si>
+    <t>Current CTC</t>
+  </si>
+  <si>
+    <t>Expected CTC</t>
+  </si>
+  <si>
+    <t>OfferLetter Msg</t>
+  </si>
+  <si>
+    <t>messageFor TL</t>
+  </si>
+  <si>
+    <t>finalStatus</t>
+  </si>
+  <si>
+    <t>Interviewdate</t>
+  </si>
+  <si>
+    <t>InterviewTime</t>
+  </si>
+  <si>
+    <t>rani</t>
+  </si>
+  <si>
+    <t>918080888889</t>
+  </si>
+  <si>
+    <t>Eligible</t>
+  </si>
+  <si>
+    <t>23123123119</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Backend Developer </t>
+  </si>
+  <si>
+    <t>Infosys</t>
+  </si>
+  <si>
+    <t>mumbai</t>
+  </si>
+  <si>
+    <t>Degree In CS</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2 year,8 month</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>7 Lakh, Thousand</t>
+  </si>
+  <si>
+    <t>10 Lakh, Thousand</t>
+  </si>
+  <si>
+    <t>APPLICANT NAME</t>
+  </si>
+  <si>
+    <t>CONTACT NUMBER</t>
+  </si>
+  <si>
+    <t>PREFFERED LOCATION</t>
+  </si>
+  <si>
+    <t>RUTUJA</t>
+  </si>
+  <si>
+    <t>MUMBAI</t>
+  </si>
+  <si>
+    <t>NOTICE PERIOD</t>
+  </si>
+  <si>
+    <t>60 DAYS</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>rutuja99@gmail.com</t>
+  </si>
+  <si>
+    <t>CERTIFICATION</t>
+  </si>
+  <si>
+    <t>SQL,REACT JS</t>
+  </si>
+  <si>
+    <t>CTC</t>
+  </si>
+  <si>
+    <t>2 lakhs,50 thousand</t>
+  </si>
+  <si>
+    <t>EXP_CTC</t>
+  </si>
+  <si>
+    <t>4 lakhs, 0 thousand</t>
+  </si>
+  <si>
+    <t>EDUCATION</t>
+  </si>
+  <si>
+    <t>BSC</t>
+  </si>
+  <si>
+    <t>JOBDESIGNATION</t>
+  </si>
+  <si>
+    <t>reactJS developer</t>
+  </si>
+  <si>
+    <t>CURRENT LOCATION</t>
+  </si>
+  <si>
+    <t>PUNE</t>
+  </si>
+  <si>
+    <t>TOTAL EXPERIENCE</t>
+  </si>
+  <si>
+    <t>RELEVENT EXP</t>
+  </si>
+  <si>
+    <t>2 YEAR,8 MONTHS</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>OFFER LETTER</t>
+  </si>
+  <si>
+    <t>COMPANY NAME</t>
+  </si>
+  <si>
+    <t>OFFER SALARY</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>OFFER DETAILS</t>
+  </si>
+  <si>
+    <t>1 YEAR BOND</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>COMPANY CULTURE</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>BASED ON THE IMPORTANCE</t>
   </si>
 </sst>
 </file>
@@ -464,12 +682,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -480,6 +697,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -769,29 +993,29 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="14.42578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="5" max="5" customWidth="true" width="12.42578125"/>
-    <col min="6" max="6" customWidth="true" width="11.7109375"/>
-    <col min="7" max="7" customWidth="true" width="20.140625"/>
-    <col min="10" max="10" customWidth="true" width="9.85546875"/>
-    <col min="11" max="11" customWidth="true" width="14.140625"/>
-    <col min="12" max="12" customWidth="true" width="12.28515625"/>
-    <col min="13" max="13" customWidth="true" width="13.5703125"/>
-    <col min="14" max="14" customWidth="true" width="11.85546875"/>
-    <col min="15" max="15" customWidth="true" width="12.0"/>
-    <col min="16" max="16" customWidth="true" width="14.42578125"/>
-    <col min="17" max="17" customWidth="true" width="10.85546875"/>
-    <col min="18" max="18" customWidth="true" width="11.85546875"/>
-    <col min="19" max="19" customWidth="true" width="10.42578125"/>
-    <col min="20" max="20" customWidth="true" width="23.0"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -855,13 +1079,13 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="9" t="s">
         <v>77</v>
       </c>
     </row>
@@ -869,7 +1093,7 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -932,7 +1156,7 @@
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -968,67 +1192,67 @@
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>3232132321</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5">
         <v>1</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>2</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>1</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="6">
         <v>240000</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>300000</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="S4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="11">
+      <c r="U4" s="10">
         <v>37644</v>
       </c>
       <c r="V4" s="1"/>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="11" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1073,211 +1297,211 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection sqref="A1:AB5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.7109375"/>
-    <col min="2" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="12.7109375"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375"/>
-    <col min="5" max="5" customWidth="true" width="13.42578125"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875"/>
-    <col min="7" max="7" customWidth="true" width="11.85546875"/>
-    <col min="8" max="8" customWidth="true" width="16.140625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
-    <col min="11" max="11" customWidth="true" width="13.7109375"/>
-    <col min="12" max="12" customWidth="true" width="12.5703125"/>
-    <col min="14" max="14" customWidth="true" width="14.5703125"/>
-    <col min="15" max="15" customWidth="true" width="18.28515625"/>
-    <col min="16" max="16" customWidth="true" width="13.140625"/>
-    <col min="17" max="17" customWidth="true" width="11.7109375"/>
-    <col min="18" max="18" customWidth="true" width="12.140625"/>
-    <col min="19" max="19" customWidth="true" width="20.7109375"/>
-    <col min="20" max="20" customWidth="true" width="11.0"/>
-    <col min="21" max="21" customWidth="true" width="13.0"/>
-    <col min="22" max="22" customWidth="true" width="11.42578125"/>
-    <col min="23" max="23" customWidth="true" width="19.140625"/>
-    <col min="24" max="24" customWidth="true" width="15.5703125"/>
-    <col min="25" max="25" customWidth="true" width="26.7109375"/>
-    <col min="26" max="26" customWidth="true" width="19.42578125"/>
-    <col min="27" max="27" customWidth="true" width="14.85546875"/>
-    <col min="28" max="28" customWidth="true" width="14.0"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="25" max="25" width="26.7109375" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>92</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
         <v>94</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>97</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>95</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" t="s" s="0">
+      <c r="Q2" t="s">
         <v>87</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="R2" t="s">
         <v>88</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>79</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>89</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>90</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>29</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>81</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" t="s" s="0">
+      <c r="Z2" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" t="s" s="0">
+      <c r="AA2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="1">
@@ -1294,7 +1518,7 @@
       <c r="H3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>36809</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1342,6 +1566,598 @@
         <v>38</v>
       </c>
       <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
+        <v>100</v>
+      </c>
+      <c r="U2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2312312311</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2022</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T2" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>2024</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1">
+        <v>15</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
@@ -1414,242 +2230,237 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A2:AF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="8" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M2" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="8" t="s">
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="P2" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="Q2" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="8" t="s">
+      <c r="R2" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" t="s">
+        <v>124</v>
+      </c>
+      <c r="T2" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" t="s">
+        <v>127</v>
+      </c>
+      <c r="W2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y2" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="Z2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF2" s="15"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="M2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="N2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="Q2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="R2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="T2" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="U2" t="s" s="0">
-        <v>100</v>
-      </c>
-      <c r="V2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="W2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="X2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="Y2" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="Z2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="AA2" t="s" s="0">
-        <v>71</v>
-      </c>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" t="s">
+        <v>143</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" t="s">
+        <v>146</v>
+      </c>
+      <c r="T3" t="s">
+        <v>147</v>
+      </c>
+      <c r="U3" t="s">
+        <v>148</v>
+      </c>
+      <c r="V3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" t="s">
+        <v>149</v>
+      </c>
+      <c r="X3" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF3" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2312312311</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2022</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1678,296 +2489,12 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
     </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>112</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>85</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="M2" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="N2" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="Q2" t="s" s="0">
-        <v>87</v>
-      </c>
-      <c r="R2" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>79</v>
-      </c>
-      <c r="T2" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="U2" t="s" s="0">
-        <v>90</v>
-      </c>
-      <c r="V2" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="W2" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="X2" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="Y2" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="Z2" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="AA2" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="AB2" s="0"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1">
-        <v>2024</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>3</v>
-      </c>
-      <c r="R3" s="1">
-        <v>15</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1996,10 +2523,214 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" t="s">
+        <v>172</v>
+      </c>
+      <c r="N1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" t="s">
+        <v>175</v>
+      </c>
+      <c r="P1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>177</v>
+      </c>
+      <c r="R1" t="s">
+        <v>178</v>
+      </c>
+      <c r="S1" t="s">
+        <v>180</v>
+      </c>
+      <c r="T1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2">
+        <v>8989898989</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L2" t="s">
+        <v>171</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>179</v>
+      </c>
+      <c r="R2">
+        <v>3.6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>181</v>
+      </c>
+      <c r="T2" t="s">
+        <v>183</v>
+      </c>
+      <c r="U2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
base url updated and applicant
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\Recruiter\Recruiter_Gears\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6180" firstSheet="3" activeTab="5"/>
   </bookViews>
@@ -15,7 +20,6 @@
     <sheet name="applicant" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="187">
   <si>
     <t>source</t>
   </si>
@@ -583,6 +587,9 @@
   </si>
   <si>
     <t>BASED ON THE IMPORTANCE</t>
+  </si>
+  <si>
+    <t>2 YEAR,6 MONTHS</t>
   </si>
 </sst>
 </file>
@@ -2570,10 +2577,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2699,8 +2706,8 @@
       <c r="L2" t="s">
         <v>171</v>
       </c>
-      <c r="M2">
-        <v>2</v>
+      <c r="M2" t="s">
+        <v>186</v>
       </c>
       <c r="N2" t="s">
         <v>174</v>
@@ -2727,7 +2734,6 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
salary calculation and copy link
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="188">
   <si>
     <t>source</t>
   </si>
@@ -590,6 +590,9 @@
   </si>
   <si>
     <t>CALL AFTER SOME TIME</t>
+  </si>
+  <si>
+    <t>2.4</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1013,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,11 +1254,11 @@
       <c r="O4" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="P4" s="20">
-        <v>240000</v>
-      </c>
-      <c r="Q4" s="20">
-        <v>300000</v>
+      <c r="P4" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
copy link-open in new tab-fill the applicant form-data flow in calling tracker
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="189">
   <si>
     <t>source</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>2.4</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1016,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,8 +1146,8 @@
       <c r="L2" s="19">
         <v>6</v>
       </c>
-      <c r="M2" s="19">
-        <v>2</v>
+      <c r="M2" s="19" t="s">
+        <v>188</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
recruiter profile -team performance
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6180" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="200">
   <si>
     <t>source</t>
   </si>
@@ -235,9 +235,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Interview Schedule</t>
-  </si>
-  <si>
     <t>DOB</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>wipro</t>
   </si>
   <si>
-    <t>rahu</t>
-  </si>
-  <si>
     <t>2 year,6 month</t>
   </si>
   <si>
@@ -289,9 +283,6 @@
     <t>1233211238</t>
   </si>
   <si>
-    <t>0010-02-26</t>
-  </si>
-  <si>
     <t>rani123@yahoo.com</t>
   </si>
   <si>
@@ -307,9 +298,6 @@
     <t>2024</t>
   </si>
   <si>
-    <t>take it</t>
-  </si>
-  <si>
     <t>raja10@gmail.com</t>
   </si>
   <si>
@@ -334,9 +322,6 @@
     <t>0022-09-19</t>
   </si>
   <si>
-    <t>rani123#@yahoo.com</t>
-  </si>
-  <si>
     <t>Candidate Name</t>
   </si>
   <si>
@@ -586,15 +571,6 @@
     <t>60 - Oracle PLSQL Developer</t>
   </si>
   <si>
-    <t>rahul@gmail.com</t>
-  </si>
-  <si>
-    <t>2323232323</t>
-  </si>
-  <si>
-    <t>others</t>
-  </si>
-  <si>
     <t>2 year,7 month</t>
   </si>
   <si>
@@ -632,6 +608,27 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>9123456789</t>
+  </si>
+  <si>
+    <t>Tech Solutions Ltd.</t>
+  </si>
+  <si>
+    <t>Candidate available for immediate joining</t>
+  </si>
+  <si>
+    <t>2000-07-15</t>
+  </si>
+  <si>
+    <t>63 - APS Core Testing</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>Krios Info Solutions Private Limited</t>
   </si>
 </sst>
 </file>
@@ -737,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -751,7 +748,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1048,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,13 +1057,13 @@
     <col min="6" max="6" customWidth="true" width="11.7109375"/>
     <col min="7" max="7" customWidth="true" width="20.140625"/>
     <col min="10" max="10" customWidth="true" width="9.85546875"/>
-    <col min="11" max="11" customWidth="true" style="18" width="12.28515625"/>
-    <col min="12" max="12" customWidth="true" style="18" width="13.5703125"/>
-    <col min="13" max="13" customWidth="true" style="18" width="11.85546875"/>
+    <col min="11" max="11" customWidth="true" style="17" width="12.28515625"/>
+    <col min="12" max="12" customWidth="true" style="17" width="13.5703125"/>
+    <col min="13" max="13" customWidth="true" style="17" width="11.85546875"/>
     <col min="14" max="14" customWidth="true" width="12.0"/>
     <col min="15" max="15" customWidth="true" width="14.42578125"/>
-    <col min="16" max="16" customWidth="true" style="18" width="10.85546875"/>
-    <col min="17" max="17" customWidth="true" style="18" width="11.85546875"/>
+    <col min="16" max="16" customWidth="true" style="17" width="10.85546875"/>
+    <col min="17" max="17" customWidth="true" style="17" width="11.85546875"/>
     <col min="18" max="18" customWidth="true" width="10.42578125"/>
     <col min="19" max="19" customWidth="true" width="23.0"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="10.42578125"/>
@@ -1132,21 +1128,21 @@
         <v>17</v>
       </c>
       <c r="T1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="W1" s="8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>19</v>
@@ -1161,10 +1157,10 @@
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>22</v>
@@ -1175,25 +1171,25 @@
       <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="15">
         <v>3</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="15">
         <v>6</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>181</v>
+      <c r="M2" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="P2" s="16">
+        <v>170</v>
+      </c>
+      <c r="P2" s="15">
         <v>3.7</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2" s="15">
         <v>5</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1226,7 +1222,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>40</v>
@@ -1266,10 +1262,10 @@
         <v>3232132321</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>40</v>
@@ -1281,39 +1277,39 @@
       <c r="J4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="16">
         <v>1</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <v>2</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <v>1</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>81</v>
+        <v>171</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="19" t="s">
-        <v>177</v>
+      <c r="S4" s="18" t="s">
+        <v>172</v>
       </c>
       <c r="T4" s="9">
         <v>37644</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W4" s="10" t="s">
         <v>26</v>
@@ -1361,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1432,7 @@
         <v>51</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>53</v>
@@ -1483,91 +1479,94 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>101</v>
+        <v>65</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>84</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>65</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>35</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>79</v>
+        <v>198</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>80</v>
+        <v>199</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>36</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="J2" t="s" s="0">
         <v>65</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="L2" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="M2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="M2" t="s" s="0">
-        <v>91</v>
-      </c>
       <c r="N2" t="s" s="0">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>65</v>
+        <v>194</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q2" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="T2" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="U2" t="s" s="0">
         <v>82</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="T2" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="U2" t="s" s="0">
-        <v>84</v>
       </c>
       <c r="V2" t="s" s="0">
         <v>26</v>
       </c>
       <c r="W2" t="s" s="0">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X2" t="s" s="0">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="Y2" t="s" s="0">
         <v>34</v>
       </c>
       <c r="Z2" t="s" s="0">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="AA2" t="s" s="0">
         <v>65</v>
       </c>
+      <c r="AB2" s="0"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B3" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1">
         <v>123321123</v>
@@ -1577,7 +1576,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
@@ -1591,17 +1590,17 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M3" s="1">
         <v>2024</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q3" s="1">
         <v>3</v>
@@ -1610,27 +1609,29 @@
         <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="1"/>
+      <c r="Z3" t="s" s="0">
+        <v>27</v>
+      </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
@@ -1708,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M11" sqref="F11:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,7 +1785,7 @@
         <v>51</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>53</v>
@@ -1834,10 +1835,10 @@
         <v>65</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>65</v>
@@ -1846,10 +1847,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>21</v>
@@ -1858,16 +1859,16 @@
         <v>65</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>65</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="N2" t="s" s="0">
         <v>65</v>
@@ -1876,22 +1877,22 @@
         <v>65</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="Q2" t="s" s="0">
         <v>65</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="S2" t="s" s="0">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="T2" t="s" s="0">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="U2" t="s" s="0">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="V2" t="s" s="0">
         <v>26</v>
@@ -1911,14 +1912,13 @@
       <c r="AA2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AB2" s="0"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1">
         <v>2312312311</v>
@@ -1932,15 +1932,15 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s" s="0">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M3" s="1">
         <v>2022</v>
@@ -1953,7 +1953,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -1965,7 +1965,7 @@
         <v>25</v>
       </c>
       <c r="Y3" t="s" s="0">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>27</v>
@@ -2116,10 +2116,10 @@
         <v>33</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>65</v>
@@ -2128,16 +2128,16 @@
         <v>35</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>36</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s" s="0">
         <v>65</v>
@@ -2146,43 +2146,43 @@
         <v>65</v>
       </c>
       <c r="L2" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="M2" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="M2" t="s" s="0">
-        <v>91</v>
-      </c>
       <c r="N2" t="s" s="0">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O2" t="s" s="0">
         <v>65</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q2" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="T2" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="U2" t="s" s="0">
         <v>82</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="T2" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="U2" t="s" s="0">
-        <v>84</v>
       </c>
       <c r="V2" t="s" s="0">
         <v>26</v>
       </c>
       <c r="W2" t="s" s="0">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="X2" t="s" s="0">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Y2" t="s" s="0">
         <v>34</v>
@@ -2199,7 +2199,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2221,11 +2221,11 @@
         <v>2024</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q3" s="1">
         <v>3</v>
@@ -2234,22 +2234,22 @@
         <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>34</v>
@@ -2372,46 +2372,46 @@
   <sheetData>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="G2" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="H2" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="I2" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="J2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="K2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="L2" t="s" s="0">
         <v>108</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="J2" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>112</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>113</v>
       </c>
       <c r="M2" t="s" s="0">
         <v>49</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="O2" t="s" s="0">
         <v>9</v>
@@ -2423,58 +2423,58 @@
         <v>52</v>
       </c>
       <c r="R2" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="T2" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="U2" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="W2" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="X2" t="s" s="0">
         <v>116</v>
-      </c>
-      <c r="T2" t="s" s="0">
-        <v>117</v>
-      </c>
-      <c r="U2" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="V2" t="s" s="0">
-        <v>119</v>
-      </c>
-      <c r="W2" t="s" s="0">
-        <v>120</v>
-      </c>
-      <c r="X2" t="s" s="0">
-        <v>121</v>
       </c>
       <c r="Y2" t="s" s="0">
         <v>58</v>
       </c>
       <c r="Z2" t="s" s="0">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AA2" t="s" s="0">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AB2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="AC2" t="s" s="0">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AD2" t="s" s="0">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AE2" t="s" s="0">
-        <v>126</v>
-      </c>
-      <c r="AF2" s="14"/>
+        <v>121</v>
+      </c>
+      <c r="AF2" s="13"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>19</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>65</v>
@@ -2483,16 +2483,16 @@
         <v>20</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J3" t="s" s="0">
         <v>65</v>
@@ -2510,10 +2510,10 @@
         <v>65</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="Q3" t="s" s="0">
         <v>65</v>
@@ -2522,22 +2522,22 @@
         <v>65</v>
       </c>
       <c r="S3" t="s" s="0">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="T3" t="s" s="0">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="U3" t="s" s="0">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="V3" t="s" s="0">
         <v>25</v>
       </c>
       <c r="W3" t="s" s="0">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="X3" t="s" s="0">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="Y3" t="s" s="0">
         <v>39</v>
@@ -2702,117 +2702,117 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B2" s="10">
         <v>8989898989</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G2" s="11">
         <v>36825</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>67</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>26</v>
@@ -2821,13 +2821,13 @@
         <v>3.6</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="T2" s="10">
         <v>123321123</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
profile section and helpinterviewQuestion
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\Recruiter\Recruiter_Gears\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6180" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AddCandidate" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="lineUpTracker" sheetId="5" r:id="rId4"/>
     <sheet name="Hold Candidate" sheetId="6" r:id="rId5"/>
     <sheet name="applicant" sheetId="7" r:id="rId6"/>
+    <sheet name="InterViewQuestion" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="209">
   <si>
     <t>source</t>
   </si>
@@ -629,6 +630,33 @@
   </si>
   <si>
     <t>Krios Info Solutions Private Limited</t>
+  </si>
+  <si>
+    <t>job id</t>
+  </si>
+  <si>
+    <t>InterViewRound</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>23 : 157 Industries Pvt Ltd</t>
+  </si>
+  <si>
+    <t>HR Round</t>
+  </si>
+  <si>
+    <t>what is the work of recruiter</t>
+  </si>
+  <si>
+    <t>Technical Round</t>
+  </si>
+  <si>
+    <t>110 : Krios Info Solutions Private Limited</t>
+  </si>
+  <si>
+    <t>what is the full form of ERP?</t>
   </si>
 </sst>
 </file>
@@ -692,7 +720,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -702,6 +730,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -756,6 +790,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1050,23 +1085,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="14.42578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="5" max="5" customWidth="true" width="12.42578125"/>
-    <col min="6" max="6" customWidth="true" width="11.7109375"/>
-    <col min="7" max="7" customWidth="true" width="20.140625"/>
-    <col min="10" max="10" customWidth="true" width="9.85546875"/>
-    <col min="11" max="11" customWidth="true" style="17" width="12.28515625"/>
-    <col min="12" max="12" customWidth="true" style="17" width="13.5703125"/>
-    <col min="13" max="13" customWidth="true" style="17" width="11.85546875"/>
-    <col min="14" max="14" customWidth="true" width="12.0"/>
-    <col min="15" max="15" customWidth="true" width="14.42578125"/>
-    <col min="16" max="16" customWidth="true" style="17" width="10.85546875"/>
-    <col min="17" max="17" customWidth="true" style="17" width="11.85546875"/>
-    <col min="18" max="18" customWidth="true" width="10.42578125"/>
-    <col min="19" max="19" customWidth="true" width="23.0"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="17" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="17" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="17" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="19" max="19" width="23" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -1357,38 +1392,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.7109375"/>
-    <col min="2" max="2" customWidth="true" width="18.140625"/>
-    <col min="3" max="3" customWidth="true" width="12.7109375"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375"/>
-    <col min="5" max="5" customWidth="true" width="13.42578125"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875"/>
-    <col min="7" max="7" customWidth="true" width="11.85546875"/>
-    <col min="8" max="8" customWidth="true" width="16.140625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
-    <col min="11" max="11" customWidth="true" width="13.7109375"/>
-    <col min="12" max="12" customWidth="true" width="12.5703125"/>
-    <col min="14" max="14" customWidth="true" width="14.5703125"/>
-    <col min="15" max="15" customWidth="true" width="18.28515625"/>
-    <col min="16" max="16" customWidth="true" width="13.140625"/>
-    <col min="17" max="17" customWidth="true" width="11.7109375"/>
-    <col min="18" max="18" customWidth="true" width="12.140625"/>
-    <col min="19" max="19" customWidth="true" width="20.7109375"/>
-    <col min="20" max="20" customWidth="true" width="11.0"/>
-    <col min="21" max="21" customWidth="true" width="13.0"/>
-    <col min="22" max="22" customWidth="true" width="11.42578125"/>
-    <col min="23" max="23" customWidth="true" width="19.140625"/>
-    <col min="24" max="24" customWidth="true" width="15.5703125"/>
-    <col min="25" max="25" customWidth="true" width="26.7109375"/>
-    <col min="26" max="26" customWidth="true" width="19.42578125"/>
-    <col min="27" max="27" customWidth="true" width="14.85546875"/>
-    <col min="28" max="28" customWidth="true" width="14.0"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" customWidth="1"/>
+    <col min="25" max="25" width="26.7109375" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1478,88 +1513,87 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>193</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>198</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>199</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>196</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
         <v>195</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>85</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>88</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="O2" t="s" s="0">
+      <c r="N2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" t="s">
         <v>194</v>
       </c>
-      <c r="P2" t="s" s="0">
+      <c r="P2" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" t="s" s="0">
+      <c r="Q2" t="s">
         <v>79</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="R2" t="s">
         <v>80</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>192</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>81</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>82</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>74</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>87</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" t="s" s="0">
+      <c r="Z2" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="AB2" s="0"/>
+      <c r="AA2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1629,7 +1663,7 @@
       <c r="Y3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" t="s" s="0">
+      <c r="Z3" t="s">
         <v>27</v>
       </c>
       <c r="AA3" s="1"/>
@@ -1715,33 +1749,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.140625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.7109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.28515625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.28515625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.85546875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="7.85546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.7109375"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.28515625"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.7109375"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.42578125"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="20" max="21" bestFit="true" customWidth="true" width="18.28515625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="11.140625"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.28515625"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="24.85546875"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="14.28515625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.5703125"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1831,85 +1865,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>188</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>189</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>190</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s" s="0">
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
         <v>90</v>
       </c>
-      <c r="K2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
         <v>91</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>191</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="N2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" t="s">
         <v>180</v>
       </c>
-      <c r="Q2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="R2" t="s" s="0">
+      <c r="Q2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" t="s">
         <v>181</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>192</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>182</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>183</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="W2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="X2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="Y2" t="s" s="0">
+      <c r="W2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="AA2" t="s" s="0">
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1924,14 +1958,14 @@
         <v>2312312311</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>187</v>
       </c>
       <c r="I3" s="12"/>
@@ -1964,7 +1998,7 @@
       <c r="X3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" t="s" s="0">
+      <c r="Y3" t="s">
         <v>186</v>
       </c>
       <c r="Z3" s="1" t="s">
@@ -2022,7 +2056,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2112,85 +2146,85 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>93</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>77</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>78</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>96</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="L2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
         <v>85</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>88</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>86</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="P2" t="s" s="0">
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" t="s" s="0">
+      <c r="Q2" t="s">
         <v>79</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="R2" t="s">
         <v>80</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>72</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>81</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>82</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>94</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>87</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" t="s" s="0">
+      <c r="Z2" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" t="s" s="0">
+      <c r="AA2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2339,222 +2373,222 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.42578125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.42578125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="25.28515625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.42578125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="7.28515625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="23.42578125"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="7.85546875"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.28515625"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="38.85546875"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.85546875"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="19.5703125"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="21.42578125"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="19.28515625"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.140625"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="24.85546875"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="15.28515625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.5703125"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.42578125"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="13.7109375"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="14.140625"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>97</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>102</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>103</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>104</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>105</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>106</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>107</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>108</v>
       </c>
-      <c r="M2" t="s" s="0">
+      <c r="M2" t="s">
         <v>49</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>109</v>
       </c>
-      <c r="O2" t="s" s="0">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="P2" t="s" s="0">
+      <c r="P2" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" t="s" s="0">
+      <c r="Q2" t="s">
         <v>52</v>
       </c>
-      <c r="R2" t="s" s="0">
+      <c r="R2" t="s">
         <v>110</v>
       </c>
-      <c r="S2" t="s" s="0">
+      <c r="S2" t="s">
         <v>111</v>
       </c>
-      <c r="T2" t="s" s="0">
+      <c r="T2" t="s">
         <v>112</v>
       </c>
-      <c r="U2" t="s" s="0">
+      <c r="U2" t="s">
         <v>113</v>
       </c>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>114</v>
       </c>
-      <c r="W2" t="s" s="0">
+      <c r="W2" t="s">
         <v>115</v>
       </c>
-      <c r="X2" t="s" s="0">
+      <c r="X2" t="s">
         <v>116</v>
       </c>
-      <c r="Y2" t="s" s="0">
+      <c r="Y2" t="s">
         <v>58</v>
       </c>
-      <c r="Z2" t="s" s="0">
+      <c r="Z2" t="s">
         <v>117</v>
       </c>
-      <c r="AA2" t="s" s="0">
+      <c r="AA2" t="s">
         <v>118</v>
       </c>
-      <c r="AB2" t="s" s="0">
+      <c r="AB2" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" t="s" s="0">
+      <c r="AC2" t="s">
         <v>119</v>
       </c>
-      <c r="AD2" t="s" s="0">
+      <c r="AD2" t="s">
         <v>120</v>
       </c>
-      <c r="AE2" t="s" s="0">
+      <c r="AE2" t="s">
         <v>121</v>
       </c>
       <c r="AF2" s="13"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>122</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s" s="0">
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>124</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>125</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>126</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>127</v>
       </c>
-      <c r="J3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s" s="0">
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="N3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="O3" t="s" s="0">
+      <c r="L3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" t="s">
         <v>128</v>
       </c>
-      <c r="P3" t="s" s="0">
+      <c r="P3" t="s">
         <v>129</v>
       </c>
-      <c r="Q3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="R3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="S3" t="s" s="0">
+      <c r="Q3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" t="s">
         <v>130</v>
       </c>
-      <c r="T3" t="s" s="0">
+      <c r="T3" t="s">
         <v>131</v>
       </c>
-      <c r="U3" t="s" s="0">
+      <c r="U3" t="s">
         <v>132</v>
       </c>
-      <c r="V3" t="s" s="0">
+      <c r="V3" t="s">
         <v>25</v>
       </c>
-      <c r="W3" t="s" s="0">
+      <c r="W3" t="s">
         <v>133</v>
       </c>
-      <c r="X3" t="s" s="0">
+      <c r="X3" t="s">
         <v>134</v>
       </c>
-      <c r="Y3" t="s" s="0">
+      <c r="Y3" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="AA3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="AB3" t="s" s="0">
+      <c r="Z3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB3" t="s">
         <v>34</v>
       </c>
-      <c r="AC3" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="AD3" t="s" s="0">
+      <c r="AC3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD3" t="s">
         <v>65</v>
       </c>
       <c r="AF3" s="1"/>
@@ -2677,27 +2711,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.85546875"/>
-    <col min="2" max="2" customWidth="true" width="17.85546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.5703125"/>
-    <col min="4" max="4" customWidth="true" width="20.5703125"/>
-    <col min="5" max="5" customWidth="true" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" width="14.42578125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.5703125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.85546875"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="17.85546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.5703125"/>
-    <col min="15" max="15" customWidth="true" width="8.140625"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.140625"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.5703125"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.7109375"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.140625"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="19.42578125"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -2837,4 +2871,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>